<commit_message>
Ajustes para invocar correctamente al servicio de correspondencia.
</commit_message>
<xml_diff>
--- a/Massive-Loader-Root/upload-dir/Plantilla Cargue Contigencia-Cuba.xlsx
+++ b/Massive-Loader-Root/upload-dir/Plantilla Cargue Contigencia-Cuba.xlsx
@@ -5,22 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g2o\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Colombia\Correspondencia\repos\fab-carga-masiva\massive-loader\Massive-Loader-Root\upload-dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="19995" windowHeight="7290"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="19992" windowHeight="7296"/>
   </bookViews>
   <sheets>
     <sheet name="Contingencia Entrada" sheetId="4" r:id="rId1"/>
     <sheet name="Datos" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="109">
   <si>
     <t>No. radicado</t>
   </si>
@@ -338,6 +338,15 @@
   </si>
   <si>
     <t>1000.1000_VICEPRESIDENCIA ADMINISTRATIVA/10001000</t>
+  </si>
+  <si>
+    <t>TP-PERPN/Persona Natural</t>
+  </si>
+  <si>
+    <t>La mia</t>
+  </si>
+  <si>
+    <t>Jorge Infante</t>
   </si>
 </sst>
 </file>
@@ -776,31 +785,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="35.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="3" max="3" width="35.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.109375" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
     <col min="10" max="10" width="22" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" customWidth="1"/>
-    <col min="12" max="12" width="40.42578125" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" customWidth="1"/>
-    <col min="14" max="14" width="34.140625" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" customWidth="1"/>
-    <col min="16" max="16" width="35.85546875" customWidth="1"/>
+    <col min="11" max="11" width="16.44140625" customWidth="1"/>
+    <col min="12" max="12" width="40.44140625" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" customWidth="1"/>
+    <col min="14" max="14" width="67.21875" customWidth="1"/>
+    <col min="15" max="15" width="45.88671875" customWidth="1"/>
+    <col min="16" max="16" width="35.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>14</v>
       </c>
@@ -826,7 +835,7 @@
       </c>
       <c r="P1" s="14"/>
     </row>
-    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -876,7 +885,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>21</v>
       </c>
@@ -907,12 +916,20 @@
       <c r="J3" s="6"/>
       <c r="K3" s="5"/>
       <c r="L3" s="6"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="10"/>
-    </row>
-    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="M3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>21</v>
       </c>
@@ -943,12 +960,20 @@
       <c r="J4" s="6"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="10"/>
-    </row>
-    <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="M4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>21</v>
       </c>
@@ -976,8 +1001,25 @@
       <c r="I5" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="J5" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="M5" s="5"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>21</v>
       </c>
@@ -1004,6 +1046,23 @@
       </c>
       <c r="I6" s="5" t="s">
         <v>17</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="M6" s="5"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="P6" s="10" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1039,19 +1098,19 @@
           <x14:formula1>
             <xm:f>Datos!$C$31:$C$33</xm:f>
           </x14:formula1>
-          <xm:sqref>J3:J4</xm:sqref>
+          <xm:sqref>J3:J6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Datos!$B$38:$B$48</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M4 O3</xm:sqref>
+          <xm:sqref>M3:M6 O3:O6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Datos!$B$51:$B$83</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N4 P3:P4</xm:sqref>
+          <xm:sqref>N3:N6 P3:P6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1067,13 +1126,13 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="103.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" customWidth="1"/>
+    <col min="2" max="2" width="103.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
@@ -1081,7 +1140,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1093,7 +1152,7 @@
         <v>TP-CMCOE/Comunicación Oficial Externa Recibida</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1105,7 +1164,7 @@
         <v>TP-CMCOI/Comunicación Oficial Interna Recibida</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
@@ -1113,17 +1172,17 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
@@ -1131,17 +1190,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -1149,7 +1208,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1161,7 +1220,7 @@
         <v>TL-DOCOF/Oficio</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1173,7 +1232,7 @@
         <v>TL-DOCT/Tutela</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1185,7 +1244,7 @@
         <v>TL-DOCDP/Derecho de Petición</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1197,7 +1256,7 @@
         <v>TL-DOCII/Invitación</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1209,7 +1268,7 @@
         <v>TL-DOCDM/Demanda</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1221,7 +1280,7 @@
         <v>TL-DOCF/Factura</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1233,7 +1292,7 @@
         <v>TL-DOCIE/Investigación</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1245,7 +1304,7 @@
         <v>TL-DOCDN/Denuncia</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -1257,7 +1316,7 @@
         <v>TL-DOCR/Recurso</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -1269,7 +1328,7 @@
         <v>TL-DOCP/PQRSD</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1281,7 +1340,7 @@
         <v>TL-DOCA/Acta</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -1293,7 +1352,7 @@
         <v>TL-DOCC/Circular</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -1305,7 +1364,7 @@
         <v>TL-DOCM/Memorando</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>7</v>
       </c>
@@ -1313,7 +1372,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -1325,7 +1384,7 @@
         <v>TP-PERPN/Persona Natural</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -1337,7 +1396,7 @@
         <v>TP-PERA/Anonimo</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>57</v>
       </c>
@@ -1349,15 +1408,15 @@
         <v>TP-PERPJ/Persona Jurídica</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1040</v>
       </c>
@@ -1365,7 +1424,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>200</v>
       </c>
@@ -1373,7 +1432,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>300</v>
       </c>
@@ -1381,7 +1440,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>400</v>
       </c>
@@ -1389,7 +1448,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>500</v>
       </c>
@@ -1397,7 +1456,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>600</v>
       </c>
@@ -1405,7 +1464,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>700</v>
       </c>
@@ -1413,7 +1472,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>800</v>
       </c>
@@ -1421,7 +1480,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>900</v>
       </c>
@@ -1429,7 +1488,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>100</v>
       </c>
@@ -1437,7 +1496,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1000</v>
       </c>
@@ -1445,12 +1504,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B50" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>10401040</v>
       </c>
@@ -1458,7 +1517,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>10401041</v>
       </c>
@@ -1466,7 +1525,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>10401042</v>
       </c>
@@ -1474,7 +1533,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>200210</v>
       </c>
@@ -1482,7 +1541,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>200220</v>
       </c>
@@ -1490,7 +1549,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>200230</v>
       </c>
@@ -1498,7 +1557,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>200240</v>
       </c>
@@ -1506,7 +1565,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>300310</v>
       </c>
@@ -1514,7 +1573,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>300320</v>
       </c>
@@ -1522,7 +1581,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>300330</v>
       </c>
@@ -1530,7 +1589,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>300340</v>
       </c>
@@ -1538,7 +1597,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>400410</v>
       </c>
@@ -1546,7 +1605,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>400420</v>
       </c>
@@ -1554,7 +1613,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>400430</v>
       </c>
@@ -1562,7 +1621,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>500510</v>
       </c>
@@ -1570,7 +1629,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>500520</v>
       </c>
@@ -1578,7 +1637,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>700700</v>
       </c>
@@ -1586,7 +1645,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>700710</v>
       </c>
@@ -1594,7 +1653,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>700720</v>
       </c>
@@ -1602,7 +1661,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>700730</v>
       </c>
@@ -1610,7 +1669,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>800810</v>
       </c>
@@ -1618,7 +1677,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>800820</v>
       </c>
@@ -1626,7 +1685,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>900910</v>
       </c>
@@ -1634,7 +1693,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>900920</v>
       </c>
@@ -1642,7 +1701,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>100110</v>
       </c>
@@ -1650,7 +1709,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>100120</v>
       </c>
@@ -1658,7 +1717,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>100130</v>
       </c>
@@ -1666,7 +1725,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>100100</v>
       </c>
@@ -1674,7 +1733,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>10001010</v>
       </c>
@@ -1682,7 +1741,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>10001020</v>
       </c>
@@ -1690,7 +1749,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>10001030</v>
       </c>
@@ -1698,7 +1757,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>10001040</v>
       </c>
@@ -1706,7 +1765,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>10001000</v>
       </c>
@@ -1714,19 +1773,19 @@
         <v>105</v>
       </c>
     </row>
-    <row r="299" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="299" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B299" s="2"/>
     </row>
-    <row r="311" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="311" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B311" s="2"/>
     </row>
-    <row r="317" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="317" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B317" s="2"/>
     </row>
-    <row r="566" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="566" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B566" s="2"/>
     </row>
-    <row r="601" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="601" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B601" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MOD: se ajusta el JSON  a mandar. MOD: se queman los datos que se deben obtener del servicio de regla mientras este se termina de ajustar.
</commit_message>
<xml_diff>
--- a/Massive-Loader-Root/upload-dir/Plantilla Cargue Contigencia-Cuba.xlsx
+++ b/Massive-Loader-Root/upload-dir/Plantilla Cargue Contigencia-Cuba.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="112">
   <si>
     <t>No. radicado</t>
   </si>
@@ -347,6 +347,15 @@
   </si>
   <si>
     <t>Jorge Infante</t>
+  </si>
+  <si>
+    <t>12EE2016420100000900168</t>
+  </si>
+  <si>
+    <t>12EE2016420100000900169</t>
+  </si>
+  <si>
+    <t>12EE2016420100000900170</t>
   </si>
 </sst>
 </file>
@@ -785,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -885,7 +894,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>21</v>
       </c>
@@ -929,9 +938,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="B4" s="9">
         <v>42502.916666666664</v>
@@ -973,9 +982,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>21</v>
+        <v>110</v>
       </c>
       <c r="B5" s="9">
         <v>42502.916666666664</v>
@@ -1019,9 +1028,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
       <c r="B6" s="9">
         <v>42502.916666666664</v>

</xml_diff>

<commit_message>
ajuste de plantilla de prueba
</commit_message>
<xml_diff>
--- a/Massive-Loader-Root/upload-dir/Plantilla Cargue Contigencia-Cuba.xlsx
+++ b/Massive-Loader-Root/upload-dir/Plantilla Cargue Contigencia-Cuba.xlsx
@@ -795,7 +795,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1131,7 +1131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C601"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
MOD: se dshabilita la tarea programada y se implementa un mecanismo de reintentos con spring retry. MOD: se ajustan las clases para pasar por el sonar. TODO: externalizar los parametros de reintentos.
</commit_message>
<xml_diff>
--- a/Massive-Loader-Root/upload-dir/Plantilla Cargue Contigencia-Cuba.xlsx
+++ b/Massive-Loader-Root/upload-dir/Plantilla Cargue Contigencia-Cuba.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Colombia\Correspondencia\repos\fab-carga-masiva\massive-loader\Massive-Loader-Root\upload-dir\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\loadExcelCorrespondenciaData\Massive-Loader-Root\upload-dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="106">
   <si>
     <t>No. radicado</t>
   </si>
@@ -338,24 +338,6 @@
   </si>
   <si>
     <t>1000.1000_VICEPRESIDENCIA ADMINISTRATIVA/10001000</t>
-  </si>
-  <si>
-    <t>TP-PERPN/Persona Natural</t>
-  </si>
-  <si>
-    <t>La mia</t>
-  </si>
-  <si>
-    <t>Jorge Infante</t>
-  </si>
-  <si>
-    <t>12EE2016420100000900168</t>
-  </si>
-  <si>
-    <t>12EE2016420100000900169</t>
-  </si>
-  <si>
-    <t>12EE2016420100000900170</t>
   </si>
 </sst>
 </file>
@@ -795,7 +777,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -938,141 +920,59 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" s="9">
-        <v>42502.916666666664</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="6">
-        <v>1</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>17</v>
-      </c>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
       <c r="J4" s="6"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
-      <c r="M4" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="P4" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B5" s="9">
-        <v>42502.916666666664</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="6">
-        <v>1</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>108</v>
-      </c>
+      <c r="M4" s="5"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="10"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="10"/>
-      <c r="O5" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="P5" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B6" s="9">
-        <v>42502.916666666664</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>108</v>
-      </c>
+      <c r="O5" s="5"/>
+      <c r="P5" s="10"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
       <c r="M6" s="5"/>
       <c r="N6" s="10"/>
-      <c r="O6" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="P6" s="10" t="s">
-        <v>75</v>
-      </c>
+      <c r="O6" s="5"/>
+      <c r="P6" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>